<commit_message>
implement storage, add extra field to sample mutatation
</commit_message>
<xml_diff>
--- a/tests/stubs/imports/sample.xlsx
+++ b/tests/stubs/imports/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sparclex/code/nova/tests/stubs/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B22E0F7-F8EE-6E48-88B3-98CEEC7FB10D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C83C95-A975-3544-B377-31F49840DA5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -56,17 +56,35 @@
   </si>
   <si>
     <t>Blood</t>
+  </si>
+  <si>
+    <t>XYZ124</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>extra_test</t>
+  </si>
+  <si>
+    <t>second</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -396,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -408,7 +427,7 @@
     <col min="3" max="3" width="22.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,8 +455,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -459,6 +481,37 @@
       <c r="I2">
         <v>2</v>
       </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43427</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43427</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>